<commit_message>
Added frontal kinetics and ICR calcs
</commit_message>
<xml_diff>
--- a/KAM_data.xlsx
+++ b/KAM_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,37 +8,50 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\Documents\GitHub\MCG4322B_Brace_Yourself\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43BDDE1F-EC9B-4A50-8E5D-025DA28EFF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84833B8B-0FD5-40D3-BE03-C5BB6137EC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Knee OA KAM" sheetId="1" r:id="rId1"/>
     <sheet name="Healthy KAM" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Gait %</t>
   </si>
   <si>
     <t>KAM (Nm/kg)</t>
   </si>
+  <si>
+    <t>Closest frame</t>
+  </si>
+  <si>
+    <t>Closest Frame</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -873,1165 +886,1742 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B144"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="I92" sqref="I92"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.1070083171666201</v>
       </c>
       <c r="B2">
         <v>-2.6315596845562701E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <f>ROUND((A2/100)*70,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.8450185540691799</v>
       </c>
       <c r="B3" s="1">
         <v>-2.0913910173114799E-8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="0">ROUND((A3/100)*70,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3.1365259113678299</v>
       </c>
       <c r="B4" s="1">
         <v>-2.0913910173114799E-8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4.0590351884024196</v>
       </c>
       <c r="B5">
         <v>-5.2631988419716697E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5.1660575819435</v>
       </c>
       <c r="B6">
         <v>-2.6315596845562701E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5.7195547023395701</v>
       </c>
       <c r="B7">
         <v>6.5789263994742702E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6.0885668589780897</v>
       </c>
       <c r="B8">
         <v>1.5789512870274001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6.4575649392421397</v>
       </c>
       <c r="B9">
         <v>2.2368460183658401E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6.6420639793741598</v>
       </c>
       <c r="B10">
         <v>3.1578946267689E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6.8265630195062004</v>
       </c>
       <c r="B11">
         <v>3.9473713159781099E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7.19557517614472</v>
       </c>
       <c r="B12">
         <v>5.0000018822519199E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7.7490722965407803</v>
       </c>
       <c r="B13">
         <v>6.0526224098488103E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7.7490722965407803</v>
       </c>
       <c r="B14">
         <v>7.4999988497349401E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8.1180844531792999</v>
       </c>
       <c r="B15">
         <v>8.2894755389441493E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8.1180844531792999</v>
       </c>
       <c r="B16">
         <v>9.3420960665410294E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8.3025834933113298</v>
       </c>
       <c r="B17">
         <v>0.101315777750887</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8.4870825334433508</v>
       </c>
       <c r="B18">
         <v>0.110526314028302</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8.6715815735753807</v>
       </c>
       <c r="B19">
         <v>0.114473672377655</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>8.6715815735753807</v>
       </c>
       <c r="B20">
         <v>0.12500002823377801</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>8.8560946900818696</v>
       </c>
       <c r="B21">
         <v>0.134210514317809</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9.0405937302138906</v>
       </c>
       <c r="B22">
         <v>0.143421050595224</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>9.4095918104779397</v>
       </c>
       <c r="B23">
         <v>0.15131581748731601</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9.4095918104779397</v>
       </c>
       <c r="B24">
         <v>0.15921053418602399</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>9.4095918104779397</v>
       </c>
       <c r="B25">
         <v>0.16710525088473099</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9.7786039671164602</v>
       </c>
       <c r="B26">
         <v>0.17763160674085399</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>9.7786039671164602</v>
       </c>
       <c r="B27">
         <v>0.18289473447553101</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9.7786039671164602</v>
       </c>
       <c r="B28">
         <v>0.18947368178891499</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>9.9631030072484794</v>
       </c>
       <c r="B29">
         <v>0.19868421806632999</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10.1476020473805</v>
       </c>
       <c r="B30">
         <v>0.20921052372906901</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10.3321010875125</v>
       </c>
       <c r="B31">
         <v>0.215789471042453</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10.701113244150999</v>
       </c>
       <c r="B32">
         <v>0.22763159628389901</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10.701113244150999</v>
       </c>
       <c r="B33">
         <v>0.238157901946637</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10.701113244150999</v>
       </c>
       <c r="B34">
         <v>0.24473684926002101</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>11.0701113244151</v>
       </c>
       <c r="B35">
         <v>0.25131579657340603</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>11.0701113244151</v>
       </c>
       <c r="B36">
         <v>0.26315792181485198</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>11.623622521185601</v>
       </c>
       <c r="B37">
         <v>0.272368407898882</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>11.992620601449699</v>
       </c>
       <c r="B38">
         <v>0.28421053314032801</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>11.992620601449699</v>
       </c>
       <c r="B39">
         <v>0.29210524983903602</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>12.5461317982202</v>
       </c>
       <c r="B40">
         <v>0.30526314446580399</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>12.5461317982202</v>
       </c>
       <c r="B41">
         <v>0.31052632239386602</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>12.7306308383522</v>
       </c>
       <c r="B42">
         <v>0.32105262805660401</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>13.0996289186163</v>
       </c>
       <c r="B43">
         <v>0.32894739494869601</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>13.0996289186163</v>
       </c>
       <c r="B44">
         <v>0.339473700611434</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>13.837639155518801</v>
       </c>
       <c r="B45">
         <v>0.34605264792481899</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>14.2066372357829</v>
       </c>
       <c r="B46">
         <v>0.35526318420223402</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>14.575649392421401</v>
       </c>
       <c r="B47">
         <v>0.36447367028626498</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>15.313659629324</v>
       </c>
       <c r="B48">
         <v>0.37236843717835699</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>15.867156749719999</v>
       </c>
       <c r="B49">
         <v>0.380263153877064</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>16.4206679464906</v>
       </c>
       <c r="B50">
         <v>0.38684210119044898</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>17.158678183393199</v>
       </c>
       <c r="B51">
         <v>0.39473686808254099</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>17.896674343921301</v>
       </c>
       <c r="B52">
         <v>0.40131581539592498</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>19.188195777594402</v>
       </c>
       <c r="B53">
         <v>0.40394735416657102</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>20.110705054629001</v>
       </c>
       <c r="B54">
         <v>0.40789476270931002</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>21.5867114520596</v>
       </c>
       <c r="B55">
         <v>0.402631584781248</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>22.3247216889622</v>
       </c>
       <c r="B56">
         <v>0.39605263746786401</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>23.0627319258647</v>
       </c>
       <c r="B57">
         <v>0.39210527911851001</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>24.169740243031399</v>
       </c>
       <c r="B58">
         <v>0.38552633180512502</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>24.907750479933899</v>
       </c>
       <c r="B59">
         <v>0.380263153877064</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>25.830259756968498</v>
       </c>
       <c r="B60">
         <v>0.37500002614238698</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>26.199257837232601</v>
       </c>
       <c r="B61">
         <v>0.36973684821432601</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>27.490779270905701</v>
       </c>
       <c r="B62">
         <v>0.36447367028626498</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>28.413288547940301</v>
       </c>
       <c r="B63">
         <v>0.35921054255158802</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>29.7047959052389</v>
       </c>
       <c r="B64">
         <v>0.35263159523820298</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>30.627305182273499</v>
       </c>
       <c r="B65">
         <v>0.35131577565949601</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>32.103325656078603</v>
       </c>
       <c r="B66">
         <v>0.34868423688884997</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>33.210333973245298</v>
       </c>
       <c r="B67">
         <v>0.34605264792481899</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <f t="shared" ref="C67:C130" si="1">ROUND((A67/100)*70,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>34.686354447050398</v>
       </c>
       <c r="B68">
         <v>0.34342105896078801</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>35.977861804348997</v>
       </c>
       <c r="B69">
         <v>0.34473682834611102</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>37.453882278154197</v>
       </c>
       <c r="B70">
         <v>0.34868423688884997</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>38.560890595320799</v>
       </c>
       <c r="B71">
         <v>0.34868423688884997</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>39.852397952619398</v>
       </c>
       <c r="B72">
         <v>0.35263159523820298</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>40.774907229653998</v>
       </c>
       <c r="B73">
         <v>0.35263159523820298</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>42.250927703459197</v>
       </c>
       <c r="B74">
         <v>0.35657895358755698</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>44.095946257528297</v>
       </c>
       <c r="B75">
         <v>0.35921054255158802</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>45.018455534562897</v>
       </c>
       <c r="B76">
         <v>0.35921054255158802</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>46.309962891861602</v>
       </c>
       <c r="B77">
         <v>0.35921054255158802</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>47.601484325534699</v>
       </c>
       <c r="B78">
         <v>0.35921054255158802</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>49.446502879603898</v>
       </c>
       <c r="B79">
         <v>0.35263159523820298</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>50.184499040132003</v>
       </c>
       <c r="B80">
         <v>0.34605264792481899</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>51.291521433673097</v>
       </c>
       <c r="B81">
         <v>0.339473700611434</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>52.029517594201202</v>
       </c>
       <c r="B82">
         <v>0.33026316433401898</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>52.3985297508397</v>
       </c>
       <c r="B83">
         <v>0.31973685867128099</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>52.952026871235802</v>
       </c>
       <c r="B84">
         <v>0.313157911357897</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>53.505538068006302</v>
       </c>
       <c r="B85">
         <v>0.30263160569515901</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>53.690037108138299</v>
       </c>
       <c r="B86">
         <v>0.29342106941774299</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>54.243548304908899</v>
       </c>
       <c r="B87">
         <v>0.28026317479097401</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>54.797045425304901</v>
       </c>
       <c r="B88">
         <v>0.26973686912823602</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>54.981558541811403</v>
       </c>
       <c r="B89">
         <v>0.25657897450146699</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>55.350556622075501</v>
       </c>
       <c r="B90">
         <v>0.246052618645344</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>55.719554702339501</v>
       </c>
       <c r="B91">
         <v>0.238157901946637</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>55.904067818846002</v>
       </c>
       <c r="B92">
         <v>0.22763159628389901</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>56.273065899110001</v>
       </c>
       <c r="B93">
         <v>0.21710529062116099</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>56.273065899110001</v>
       </c>
       <c r="B94">
         <v>0.20789475434374599</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>56.826577095880602</v>
       </c>
       <c r="B95">
         <v>0.19605262910230001</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>57.011076136012598</v>
       </c>
       <c r="B96">
         <v>0.18157896509020799</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>57.380074216276697</v>
       </c>
       <c r="B97">
         <v>0.17105265942747</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>57.749086372915201</v>
       </c>
       <c r="B98">
         <v>0.15921053418602399</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>58.1180844531793</v>
       </c>
       <c r="B99">
         <v>0.148684228523285</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>58.1180844531793</v>
       </c>
       <c r="B100">
         <v>0.14078946163119299</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>58.487082533443299</v>
       </c>
       <c r="B101">
         <v>0.12894738658313201</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>58.671595649949801</v>
       </c>
       <c r="B102">
         <v>0.118421080920394</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>59.0405937302138</v>
       </c>
       <c r="B103">
         <v>0.109210544642979</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>59.409591810477899</v>
       </c>
       <c r="B104">
         <v>9.8684238980241104E-2</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C104">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>59.5941049269844</v>
       </c>
       <c r="B105">
         <v>9.0789472088148998E-2</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C105">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>59.5941049269844</v>
       </c>
       <c r="B106">
         <v>7.8947397040087797E-2</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>59.963103007248399</v>
       </c>
       <c r="B107">
         <v>7.1052630147995594E-2</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C107">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>60.332101087512498</v>
       </c>
       <c r="B108">
         <v>6.0526224098488103E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C108">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>60.516614204019</v>
       </c>
       <c r="B109">
         <v>5.2631607786550003E-2</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C109">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>60.885612284282999</v>
       </c>
       <c r="B110">
         <v>4.4736840894457897E-2</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C110">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>61.070111324415002</v>
       </c>
       <c r="B111">
         <v>3.4210485038335001E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C111">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>61.808121561317598</v>
       </c>
       <c r="B112">
         <v>2.3684229568981498E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C112">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>61.992620601449602</v>
       </c>
       <c r="B113">
         <v>1.18421043275356E-2</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C113">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>62.730630838352198</v>
       </c>
       <c r="B114">
         <v>2.6316182435051202E-3</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C114">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>63.468641075254801</v>
       </c>
       <c r="B115">
         <v>-6.5789682272946104E-3</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C115">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>64.206651312157305</v>
       </c>
       <c r="B116">
         <v>-1.3157915540679001E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C116">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>65.682657709588</v>
       </c>
       <c r="B117">
         <v>-2.1052632239386498E-2</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C117">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>66.605166986622606</v>
       </c>
       <c r="B118">
         <v>-2.6315810167447901E-2</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C118">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>68.081187460427699</v>
       </c>
       <c r="B119">
         <v>-2.36841710100326E-2</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C119">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>69.557193857858394</v>
       </c>
       <c r="B120">
         <v>-2.23684016247096E-2</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C120">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>71.033214331663601</v>
       </c>
       <c r="B121">
         <v>-2.23684016247096E-2</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C121">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>72.140222648830203</v>
       </c>
       <c r="B122">
         <v>-1.71052236966482E-2</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C122">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>73.800742162767307</v>
       </c>
       <c r="B123">
         <v>-1.1842146155356101E-2</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C123">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>74.907750479933995</v>
       </c>
       <c r="B124">
         <v>-1.05262763832637E-2</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C124">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>76.383770953739102</v>
       </c>
       <c r="B125">
         <v>-7.8947376126176604E-3</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C125">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>77.490779270905705</v>
       </c>
       <c r="B126">
         <v>-7.8947376126176604E-3</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C126">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>78.597787588072293</v>
       </c>
       <c r="B127">
         <v>-6.5789682272946104E-3</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C127">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>80.073808061877401</v>
       </c>
       <c r="B128">
         <v>-6.5789682272946104E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C128">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>81.365315419176099</v>
       </c>
       <c r="B129">
         <v>-5.2631988419716697E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C129">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>82.472323736342702</v>
       </c>
       <c r="B130">
         <v>-6.5789682272946104E-3</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C130">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>83.948344210147795</v>
       </c>
       <c r="B131">
         <v>-5.2631988419716697E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C131">
+        <f t="shared" ref="C131:C144" si="2">ROUND((A131/100)*70,0)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>85.055352527314497</v>
       </c>
       <c r="B132">
         <v>-5.2631988419716697E-3</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C132">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>85.977861804349004</v>
       </c>
       <c r="B133">
         <v>-5.2631988419716697E-3</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>87.269383238022101</v>
       </c>
       <c r="B134">
         <v>-7.8947376126176604E-3</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>88.745389635452796</v>
       </c>
       <c r="B135">
         <v>-7.8947376126176604E-3</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>90.221410109257903</v>
       </c>
       <c r="B136">
         <v>-7.8947376126176604E-3</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C136">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>91.328418426424605</v>
       </c>
       <c r="B137">
         <v>-1.05262763832637E-2</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C137">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>92.435426743591194</v>
       </c>
       <c r="B138">
         <v>-9.2105069979407199E-3</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>94.095946257528297</v>
       </c>
       <c r="B139">
         <v>-9.2105069979407199E-3</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C139">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>95.202954574694999</v>
       </c>
       <c r="B140">
         <v>-6.5789682272946104E-3</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C140">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>96.494476008368096</v>
       </c>
       <c r="B141">
         <v>-5.2631988419716697E-3</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C141">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>97.601484325534699</v>
       </c>
       <c r="B142">
         <v>-1.3157902992332101E-3</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>98.892991682833298</v>
       </c>
       <c r="B143">
         <v>3.9473876288281598E-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C143">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>100.36901215663799</v>
       </c>
       <c r="B144">
         <v>6.5789263994742702E-3</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="2"/>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2040,1149 +2630,1720 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B142"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.1070083171666201</v>
       </c>
       <c r="B2">
         <v>3.1578946267689E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <f>ROUND((A2/100)*70,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.8450185540691799</v>
       </c>
       <c r="B3">
         <v>3.1578946267689E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="0">ROUND((A3/100)*70,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2.9520268712357902</v>
       </c>
       <c r="B4">
         <v>3.1578946267689E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3.8745361482703902</v>
       </c>
       <c r="B5">
         <v>2.63157683396276E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5.1660575819435</v>
       </c>
       <c r="B6">
         <v>3.1578946267689E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5.7195547023395701</v>
       </c>
       <c r="B7">
         <v>3.8157893581073403E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6.4575649392421397</v>
       </c>
       <c r="B8">
         <v>4.7368329471719199E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6.8265630195062004</v>
       </c>
       <c r="B9">
         <v>5.5263146557196101E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6.8265630195062004</v>
       </c>
       <c r="B10">
         <v>6.31579134492882E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7.19557517614472</v>
       </c>
       <c r="B11">
         <v>7.1052630147995594E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7.19557517614472</v>
       </c>
       <c r="B12">
         <v>8.1578935810733902E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7.5645732564087602</v>
       </c>
       <c r="B13">
         <v>9.0789472088148998E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7.7490722965407803</v>
       </c>
       <c r="B14">
         <v>9.8684238980241104E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7.9335854130472798</v>
       </c>
       <c r="B15">
         <v>0.106578855292179</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8.3025834933113298</v>
       </c>
       <c r="B16">
         <v>0.114473672377655</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8.6715815735753807</v>
       </c>
       <c r="B17">
         <v>0.123684208655071</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8.8560946900818696</v>
       </c>
       <c r="B18">
         <v>0.13289464454571701</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8.8560946900818696</v>
       </c>
       <c r="B19">
         <v>0.14078946163119299</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9.0405937302138906</v>
       </c>
       <c r="B20">
         <v>0.15263148648586999</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>9.2250927703459205</v>
       </c>
       <c r="B21">
         <v>0.15921053418602399</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9.4095918104779397</v>
       </c>
       <c r="B22">
         <v>0.17105265942747</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>9.4095918104779397</v>
       </c>
       <c r="B23">
         <v>0.18289473447553101</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9.7786039671164602</v>
       </c>
       <c r="B24">
         <v>0.19078950136762299</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>9.7786039671164602</v>
       </c>
       <c r="B25">
         <v>0.201315807030361</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10.1476020473805</v>
       </c>
       <c r="B26">
         <v>0.210526343307776</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10.3321010875125</v>
       </c>
       <c r="B27">
         <v>0.22236841835583701</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10.701113244150999</v>
       </c>
       <c r="B28">
         <v>0.228947365669222</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10.701113244150999</v>
       </c>
       <c r="B29">
         <v>0.23947367133195999</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10.701113244150999</v>
       </c>
       <c r="B30">
         <v>0.25000002718808301</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>11.2546103645471</v>
       </c>
       <c r="B31">
         <v>0.260526332850821</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>11.2546103645471</v>
       </c>
       <c r="B32">
         <v>0.26973686912823602</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>11.623622521185601</v>
       </c>
       <c r="B33">
         <v>0.28026317479097401</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>11.992620601449699</v>
       </c>
       <c r="B34">
         <v>0.28947371106838998</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12.361618681713701</v>
       </c>
       <c r="B35">
         <v>0.29868419715242001</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>12.5461317982202</v>
       </c>
       <c r="B36">
         <v>0.30657896404451201</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>12.915129878484199</v>
       </c>
       <c r="B37">
         <v>0.313157911357897</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>13.0996289186163</v>
       </c>
       <c r="B38">
         <v>0.32368421702063499</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>13.653140115386799</v>
       </c>
       <c r="B39">
         <v>0.331578933719342</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>14.0221381956508</v>
       </c>
       <c r="B40">
         <v>0.33684211164740402</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>14.7601484325534</v>
       </c>
       <c r="B41">
         <v>0.34342105896078801</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>15.498158669456</v>
       </c>
       <c r="B42">
         <v>0.34868423688884997</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>16.2361689063586</v>
       </c>
       <c r="B43">
         <v>0.353947364623526</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>17.527676263657199</v>
       </c>
       <c r="B44">
         <v>0.35789472297288</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>18.265686500559799</v>
       </c>
       <c r="B45">
         <v>0.35657895358755698</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>19.372694817726401</v>
       </c>
       <c r="B46">
         <v>0.35526318420223402</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>20.295204094761001</v>
       </c>
       <c r="B47">
         <v>0.34736841731014201</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>21.2177133717956</v>
       </c>
       <c r="B48">
         <v>0.34078946999675702</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>22.3247216889622</v>
       </c>
       <c r="B49">
         <v>0.33289475329805002</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>22.693733845600701</v>
       </c>
       <c r="B50">
         <v>0.32236844763531203</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>23.431730006128799</v>
       </c>
       <c r="B51">
         <v>0.313157911357897</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>24.169740243031399</v>
       </c>
       <c r="B52">
         <v>0.30657896404451201</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>24.723251439801899</v>
       </c>
       <c r="B53">
         <v>0.294736838803066</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>25.461261676704499</v>
       </c>
       <c r="B54">
         <v>0.28815789148968202</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>25.830259756968498</v>
       </c>
       <c r="B55">
         <v>0.27631581644162101</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>26.568269993871102</v>
       </c>
       <c r="B56">
         <v>0.268421049549529</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>27.306280230773702</v>
       </c>
       <c r="B57">
         <v>0.260526332850821</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>28.0442763913017</v>
       </c>
       <c r="B58">
         <v>0.25131579657340603</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>29.151298784842801</v>
       </c>
       <c r="B59">
         <v>0.24473684926002101</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>30.073808061877401</v>
       </c>
       <c r="B60">
         <v>0.238157901946637</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>30.996317338912</v>
       </c>
       <c r="B61">
         <v>0.23421054359728299</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>32.103325656078603</v>
       </c>
       <c r="B62">
         <v>0.23157895463325301</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>33.394833013377301</v>
       </c>
       <c r="B63">
         <v>0.23026318524792999</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>34.686354447050398</v>
       </c>
       <c r="B64">
         <v>0.23026318524792999</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>35.977861804348997</v>
       </c>
       <c r="B65">
         <v>0.232894724018576</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>37.084870121515699</v>
       </c>
       <c r="B66">
         <v>0.238157901946637</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>38.376391555188803</v>
       </c>
       <c r="B67">
         <v>0.242105260295991</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <f t="shared" ref="C67:C130" si="1">ROUND((A67/100)*70,0)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>39.298900832223403</v>
       </c>
       <c r="B68">
         <v>0.24868420760937501</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>40.405909149389998</v>
       </c>
       <c r="B69">
         <v>0.25657897450146699</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>41.328418426424598</v>
       </c>
       <c r="B70">
         <v>0.260526332850821</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>42.250927703459197</v>
       </c>
       <c r="B71">
         <v>0.26973686912823602</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>43.3579360206258</v>
       </c>
       <c r="B72">
         <v>0.27499999686291299</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>44.464944337792403</v>
       </c>
       <c r="B73">
         <v>0.28026317479097401</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>45.7564657714655</v>
       </c>
       <c r="B74">
         <v>0.28421053314032801</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>46.863474088632103</v>
       </c>
       <c r="B75">
         <v>0.290789480453713</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>48.339480486062797</v>
       </c>
       <c r="B76">
         <v>0.28815789148968202</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>49.815500959867897</v>
       </c>
       <c r="B77">
         <v>0.282894763755005</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>50.738010236902497</v>
       </c>
       <c r="B78">
         <v>0.27368422747759003</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>51.660519513937103</v>
       </c>
       <c r="B79">
         <v>0.264473691200175</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>52.214030710707704</v>
       </c>
       <c r="B80">
         <v>0.25921051327211297</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>52.3985297508397</v>
       </c>
       <c r="B81">
         <v>0.247368438224052</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>53.136539987742204</v>
       </c>
       <c r="B82">
         <v>0.238157901946637</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>53.505538068006302</v>
       </c>
       <c r="B83">
         <v>0.22631577670519101</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>53.690037108138299</v>
       </c>
       <c r="B84">
         <v>0.21842106000648401</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>54.243548304908899</v>
       </c>
       <c r="B85">
         <v>0.206578934765038</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>54.243548304908899</v>
       </c>
       <c r="B86">
         <v>0.197368448681007</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>54.612546385172898</v>
       </c>
       <c r="B87">
         <v>0.188157912403592</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>54.797045425304901</v>
       </c>
       <c r="B88">
         <v>0.178947376126177</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>55.350556622075501</v>
       </c>
       <c r="B89">
         <v>0.16842107046343899</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>55.719554702339501</v>
       </c>
       <c r="B90">
         <v>0.15921053418602399</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>55.535055662207498</v>
       </c>
       <c r="B91">
         <v>0.14999999790860899</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>56.088566858978098</v>
       </c>
       <c r="B92">
         <v>0.13815792286054701</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>56.088566858978098</v>
       </c>
       <c r="B93">
         <v>0.12894738658313201</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>56.6420639793741</v>
       </c>
       <c r="B94">
         <v>0.117105261341686</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>56.826577095880602</v>
       </c>
       <c r="B95">
         <v>0.10526318629362499</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>57.195575176144601</v>
       </c>
       <c r="B96">
         <v>9.0789472088148998E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>57.5645732564087</v>
       </c>
       <c r="B97">
         <v>8.2894755389441493E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>57.5645732564087</v>
       </c>
       <c r="B98">
         <v>7.3684118725257E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>57.749086372915201</v>
       </c>
       <c r="B99">
         <v>6.31579134492882E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>57.933585413047197</v>
       </c>
       <c r="B100">
         <v>5.6578966135903699E-2</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>58.1180844531793</v>
       </c>
       <c r="B101">
         <v>4.6052660473165502E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>58.302583493311303</v>
       </c>
       <c r="B102">
         <v>3.8157893581073403E-2</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>58.671595649949801</v>
       </c>
       <c r="B103">
         <v>2.8947407497042901E-2</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>59.0405937302138</v>
       </c>
       <c r="B104">
         <v>2.10525904115661E-2</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C104">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>59.0405937302138</v>
       </c>
       <c r="B105">
         <v>9.2105655568895592E-3</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C105">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>59.5941049269844</v>
       </c>
       <c r="B106">
         <v>1.31574847141278E-3</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>59.963103007248399</v>
       </c>
       <c r="B107">
         <v>-7.8947376126176604E-3</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C107">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>60.516614204019</v>
       </c>
       <c r="B108">
         <v>-1.9736862854063501E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C108">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>61.070111324415002</v>
       </c>
       <c r="B109">
         <v>-2.7631579552770999E-2</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C109">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>62.177119641581697</v>
       </c>
       <c r="B110">
         <v>-3.1578988095509401E-2</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C110">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>63.653140115386798</v>
       </c>
       <c r="B111">
         <v>-3.1578988095509401E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C111">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>65.129160589191898</v>
       </c>
       <c r="B112">
         <v>-3.2894757480832398E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C112">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>66.420667946490596</v>
       </c>
       <c r="B113">
         <v>-2.8947348938094E-2</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C113">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>67.343177223525203</v>
       </c>
       <c r="B114">
         <v>-2.7631579552770999E-2</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C114">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>69.003696737462306</v>
       </c>
       <c r="B115">
         <v>-2.7631579552770999E-2</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C115">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>70.295204094761004</v>
       </c>
       <c r="B116">
         <v>-2.5000040782125001E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C116">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>71.586725528434101</v>
       </c>
       <c r="B117">
         <v>-2.36841710100326E-2</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C117">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>72.509234805468694</v>
       </c>
       <c r="B118">
         <v>-1.9736862854063501E-2</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C118">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>73.800742162767307</v>
       </c>
       <c r="B119">
         <v>-1.71052236966482E-2</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C119">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>74.354253359537907</v>
       </c>
       <c r="B120">
         <v>-1.1842146155356101E-2</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C120">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>75.461261676704495</v>
       </c>
       <c r="B121">
         <v>-1.1842146155356101E-2</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C121">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>76.383770953739102</v>
       </c>
       <c r="B122">
         <v>-1.1842146155356101E-2</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C122">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>77.490779270905705</v>
       </c>
       <c r="B123">
         <v>-9.2105069979407199E-3</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C123">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>78.966799744710798</v>
       </c>
       <c r="B124">
         <v>-9.2105069979407199E-3</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C124">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>80.258307102009496</v>
       </c>
       <c r="B125">
         <v>-2.6315596845562701E-3</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C125">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>81.734327575814604</v>
       </c>
       <c r="B126">
         <v>-3.9473290698793196E-3</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C126">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>83.025834933113202</v>
       </c>
       <c r="B127">
         <v>-1.3157902992332101E-3</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C127">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>83.948344210147795</v>
       </c>
       <c r="B128">
         <v>1.31574847141278E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C128">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>85.055352527314497</v>
       </c>
       <c r="B129">
         <v>1.31574847141278E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C129">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>85.977861804349004</v>
       </c>
       <c r="B130">
         <v>2.6316182435051202E-3</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C130">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>87.269383238022101</v>
       </c>
       <c r="B131">
         <v>6.5789263994742702E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C131">
+        <f t="shared" ref="C131:C142" si="2">ROUND((A131/100)*70,0)</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>88.191892515056693</v>
       </c>
       <c r="B132">
         <v>7.8946957847972309E-3</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C132">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>89.483399872355406</v>
       </c>
       <c r="B133">
         <v>1.05263349422126E-2</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>90.221410109257903</v>
       </c>
       <c r="B134">
         <v>1.31578737128587E-2</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>91.328418426424605</v>
       </c>
       <c r="B135">
         <v>1.44736430981816E-2</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>92.804438900229698</v>
       </c>
       <c r="B136">
         <v>1.7105282255597001E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C136">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>93.911447217396301</v>
       </c>
       <c r="B137">
         <v>1.8421051640920099E-2</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C137">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>94.833956494430893</v>
       </c>
       <c r="B138">
         <v>2.2368460183658401E-2</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>96.125463851729606</v>
       </c>
       <c r="B139">
         <v>1.97368210262431E-2</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C139">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>96.863474088632103</v>
       </c>
       <c r="B140">
         <v>2.10525904115661E-2</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C140">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>98.523993602569305</v>
       </c>
       <c r="B141">
         <v>2.2368460183658401E-2</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C141">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>100.184513116506</v>
       </c>
       <c r="B142">
         <v>2.3684229568981498E-2</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial logic for superior
</commit_message>
<xml_diff>
--- a/KAM_data.xlsx
+++ b/KAM_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\Documents\GitHub\MCG4322B_Brace_Yourself\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitnayak/Documents/MATLAB/MCG4322B_Brace_Yourself/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455EF6E9-57C2-4B94-83AC-2D89B87B8983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFD9E13-A862-A14D-839B-5E1DD7A735B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25360" yWindow="4900" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Knee OA KAM" sheetId="1" r:id="rId1"/>
@@ -889,17 +889,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C139" sqref="C139"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -910,7 +910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.1070083171666201</v>
       </c>
@@ -922,7 +922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.8450185540691799</v>
       </c>
@@ -934,7 +934,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3.1365259113678299</v>
       </c>
@@ -946,7 +946,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4.0590351884024196</v>
       </c>
@@ -958,7 +958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5.1660575819435</v>
       </c>
@@ -970,7 +970,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5.7195547023395701</v>
       </c>
@@ -982,7 +982,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6.0885668589780897</v>
       </c>
@@ -994,7 +994,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6.4575649392421397</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6.6420639793741598</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6.8265630195062004</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7.19557517614472</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7.7490722965407803</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7.7490722965407803</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>8.1180844531792999</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8.1180844531792999</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8.3025834933113298</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8.4870825334433508</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8.6715815735753807</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8.6715815735753807</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8.8560946900818696</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9.0405937302138906</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>9.4095918104779397</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>9.4095918104779397</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>9.4095918104779397</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>9.7786039671164602</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9.7786039671164602</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9.7786039671164602</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>9.9631030072484794</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10.1476020473805</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>10.3321010875125</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>10.701113244150999</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>10.701113244150999</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>10.701113244150999</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>11.0701113244151</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>11.0701113244151</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>11.623622521185601</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>11.992620601449699</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>11.992620601449699</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>12.5461317982202</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>12.5461317982202</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>12.7306308383522</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>13.0996289186163</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>13.0996289186163</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>13.837639155518801</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>14.2066372357829</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>14.575649392421401</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>15.313659629324</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>15.867156749719999</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>16.4206679464906</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>17.158678183393199</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>17.896674343921301</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>19.188195777594402</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>20.110705054629001</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>21.5867114520596</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>22.3247216889622</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>23.0627319258647</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>24.169740243031399</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>24.907750479933899</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>25.830259756968498</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>26.199257837232601</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>27.490779270905701</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>28.413288547940301</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>29.7047959052389</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>30.627305182273499</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>32.103325656078603</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>33.210333973245298</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>34.686354447050398</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>35.977861804348997</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>37.453882278154197</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>38.560890595320799</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>39.852397952619398</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>40.774907229653998</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>42.250927703459197</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>44.095946257528297</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>45.018455534562897</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>46.309962891861602</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>47.601484325534699</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>49.446502879603898</v>
       </c>
@@ -1842,11 +1842,11 @@
         <v>0.35263159523820298</v>
       </c>
       <c r="C79">
-        <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+        <f>ROUND((A79/100)*70,0)+27 - 1</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>50.184499040132003</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>51.291521433673097</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>52.029517594201202</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>52.3985297508397</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>52.952026871235802</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>53.505538068006302</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>53.690037108138299</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>54.243548304908899</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>54.797045425304901</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>54.981558541811403</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>55.350556622075501</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>55.719554702339501</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>55.904067818846002</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>56.273065899110001</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>56.273065899110001</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>56.826577095880602</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>57.011076136012598</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>57.380074216276697</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>57.749086372915201</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>58.1180844531793</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>58.1180844531793</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>58.487082533443299</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>58.671595649949801</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>59.0405937302138</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>59.409591810477899</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>59.5941049269844</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>59.5941049269844</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>59.963103007248399</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>60.332101087512498</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>60.516614204019</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>60.885612284282999</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>61.070111324415002</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>61.808121561317598</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>61.992620601449602</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>62.730630838352198</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>63.468641075254801</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>64.206651312157305</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>65.682657709588</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>66.605166986622606</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>68.081187460427699</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>69.557193857858394</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>71.033214331663601</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>72.140222648830203</v>
       </c>
@@ -2358,11 +2358,11 @@
         <v>-1.71052236966482E-2</v>
       </c>
       <c r="C122">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+        <f>ROUND((A122/100)*70,0)+27 + 1</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>73.800742162767307</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>74.907750479933995</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>76.383770953739102</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>77.490779270905705</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>78.597787588072293</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>80.073808061877401</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>81.365315419176099</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>82.472323736342702</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>83.948344210147795</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>85.055352527314497</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>85.977861804349004</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>87.269383238022101</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>88.745389635452796</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>90.221410109257903</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>91.328418426424605</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>92.435426743591194</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>94.095946257528297</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>95.202954574694999</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>96.494476008368096</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>97.601484325534699</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>98.892991682833298</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>100.36901215663799</v>
       </c>
@@ -2639,13 +2639,13 @@
       <selection activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.1070083171666201</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.8450185540691799</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2.9520268712357902</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3.8745361482703902</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5.1660575819435</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5.7195547023395701</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6.4575649392421397</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6.8265630195062004</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6.8265630195062004</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7.19557517614472</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7.19557517614472</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7.5645732564087602</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7.7490722965407803</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7.9335854130472798</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8.3025834933113298</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8.6715815735753807</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8.8560946900818696</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8.8560946900818696</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9.0405937302138906</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9.2250927703459205</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9.4095918104779397</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>9.4095918104779397</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>9.7786039671164602</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>9.7786039671164602</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>10.1476020473805</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>10.3321010875125</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10.701113244150999</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10.701113244150999</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10.701113244150999</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>11.2546103645471</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>11.2546103645471</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>11.623622521185601</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>11.992620601449699</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>12.361618681713701</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>12.5461317982202</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>12.915129878484199</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>13.0996289186163</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>13.653140115386799</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>14.0221381956508</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>14.7601484325534</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>15.498158669456</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>16.2361689063586</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>17.527676263657199</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>18.265686500559799</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>19.372694817726401</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>20.295204094761001</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>21.2177133717956</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>22.3247216889622</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>22.693733845600701</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>23.431730006128799</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>24.169740243031399</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>24.723251439801899</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>25.461261676704499</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>25.830259756968498</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>26.568269993871102</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>27.306280230773702</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>28.0442763913017</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>29.151298784842801</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>30.073808061877401</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>30.996317338912</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>32.103325656078603</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>33.394833013377301</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>34.686354447050398</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>35.977861804348997</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>37.084870121515699</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>38.376391555188803</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>39.298900832223403</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>40.405909149389998</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>41.328418426424598</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>42.250927703459197</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>43.3579360206258</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>44.464944337792403</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>45.7564657714655</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>46.863474088632103</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>48.339480486062797</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>49.815500959867897</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>50.738010236902497</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>51.660519513937103</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>52.214030710707704</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>52.3985297508397</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>53.136539987742204</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>53.505538068006302</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>53.690037108138299</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>54.243548304908899</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>54.243548304908899</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>54.612546385172898</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>54.797045425304901</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>55.350556622075501</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>55.719554702339501</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>55.535055662207498</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>56.088566858978098</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>56.088566858978098</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>56.6420639793741</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>56.826577095880602</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>57.195575176144601</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>57.5645732564087</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>57.5645732564087</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>57.749086372915201</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>57.933585413047197</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>58.1180844531793</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>58.302583493311303</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>58.671595649949801</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>59.0405937302138</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>59.0405937302138</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>59.5941049269844</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>59.963103007248399</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>60.516614204019</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>61.070111324415002</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>62.177119641581697</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>63.653140115386798</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>65.129160589191898</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>66.420667946490596</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>67.343177223525203</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>69.003696737462306</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>70.295204094761004</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>71.586725528434101</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>72.509234805468694</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>73.800742162767307</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>74.354253359537907</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>75.461261676704495</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>76.383770953739102</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>77.490779270905705</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>78.966799744710798</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>80.258307102009496</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>81.734327575814604</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>83.025834933113202</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>83.948344210147795</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>85.055352527314497</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>85.977861804349004</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>87.269383238022101</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>88.191892515056693</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>89.483399872355406</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>90.221410109257903</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>91.328418426424605</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>92.804438900229698</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>93.911447217396301</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>94.833956494430893</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>96.125463851729606</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>96.863474088632103</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>98.523993602569305</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>100.184513116506</v>
       </c>

</xml_diff>